<commit_message>
ph4 classification notebook code updated to be able to classify ph4s of unknown quality.
</commit_message>
<xml_diff>
--- a/data/hm_score_based_recghdata_binary.xlsx
+++ b/data/hm_score_based_recghdata_binary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livememphis-my.sharepoint.com/personal/gszwbwsk_memphis_edu/Documents/Machine Learning/ph4_classification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{C9B8850A-9A4A-4AA3-9756-4571E96154C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63CE8AB5-6A89-45B3-AC66-22332D638019}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{C9B8850A-9A4A-4AA3-9756-4571E96154C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00666B07-8C82-483B-8CB7-FF2A0265FA57}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="348" yWindow="2172" windowWidth="11460" windowHeight="9768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="score_based_ghdata_moefrags_dat" sheetId="1" r:id="rId1"/>
@@ -1015,13 +1015,13 @@
   <dimension ref="A1:AD53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T28" sqref="T27:T28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>45</v>
       </c>

</xml_diff>